<commit_message>
update opnam post data
</commit_message>
<xml_diff>
--- a/public/excel/Template Upload Opnam.xlsx
+++ b/public/excel/Template Upload Opnam.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>No</t>
   </si>
@@ -34,19 +34,10 @@
     <t>Harga Satuan</t>
   </si>
   <si>
-    <t>PCS</t>
-  </si>
-  <si>
-    <t>TEST123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing Opnam </t>
-  </si>
-  <si>
-    <t>01023-50622</t>
-  </si>
-  <si>
-    <t>BOLT, SEMS</t>
+    <t>967120Z000</t>
+  </si>
+  <si>
+    <t>HINGE LH</t>
   </si>
   <si>
     <t>Pcs</t>
@@ -97,10 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -396,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -430,47 +420,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
         <v>15000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>